<commit_message>
update pin assignments across revs
</commit_message>
<xml_diff>
--- a/Pin Assignments Accross Revs.xlsx
+++ b/Pin Assignments Accross Revs.xlsx
@@ -315,7 +315,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -338,8 +338,8 @@
   </sheetPr>
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D49" activeCellId="0" sqref="D49"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -578,7 +578,7 @@
         <v>15</v>
       </c>
       <c r="E17" s="1" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>23</v>

</xml_diff>